<commit_message>
Ad battery guard software module
</commit_message>
<xml_diff>
--- a/docs/pvz_calculations.xlsx
+++ b/docs/pvz_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projekte_JT\PVZero\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656C5FDE-3B27-4B89-A7AB-90E3A5A9F176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B13A4B-0919-4432-B2A2-451532C080A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="1725" windowWidth="28335" windowHeight="15630" xr2:uid="{D5C5EBA8-57DB-4B03-B64B-80C86E85973D}"/>
+    <workbookView xWindow="45330" yWindow="1890" windowWidth="28335" windowHeight="15630" xr2:uid="{D5C5EBA8-57DB-4B03-B64B-80C86E85973D}"/>
   </bookViews>
   <sheets>
     <sheet name="AI 0V - 60V" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>[bit]</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>OVS DEZ</t>
+  </si>
+  <si>
+    <t>OVS RAW</t>
   </si>
 </sst>
 </file>
@@ -180,9 +183,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +223,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -326,7 +329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -468,7 +471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -478,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CBA2C6-2106-4124-9378-FBEBC546B213}">
   <dimension ref="C5:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>20</v>

</xml_diff>